<commit_message>
Frontend Johan, Backend Milena documentacion Gina
</commit_message>
<xml_diff>
--- a/Documentacion/B03_Product_Backlog.xlsx
+++ b/Documentacion/B03_Product_Backlog.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mascotas\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1973B12-2F81-404D-8E0B-E72EA25201D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA9F7CA-E464-4A42-8A55-3B5FFC534777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Release Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Release Plan" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>Increment Plan</t>
   </si>
@@ -247,16 +247,7 @@
     <t>Ongoing</t>
   </si>
   <si>
-    <t>Diligenciamiento de documento IEEE 29148</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Se Desarrolla Product Backlog Priorizado</t>
-  </si>
-  <si>
-    <t>Construccion Historias de Usuario Spring 1</t>
-  </si>
-  <si>
-    <t>Configuración inicial DevOps</t>
   </si>
   <si>
     <t>Diseño mockups</t>
@@ -280,12 +271,6 @@
     <t>Codigo</t>
   </si>
   <si>
-    <t>el formulario tiene que tener los colores establecidos del proyecto</t>
-  </si>
-  <si>
-    <t>se requiere ingresar a la web</t>
-  </si>
-  <si>
     <t>Creacion de formulario Registro propietario en frontend</t>
   </si>
   <si>
@@ -296,12 +281,6 @@
   </si>
   <si>
     <t>Creacion de formulario Visita en frontend</t>
-  </si>
-  <si>
-    <t>Stack: MEVN
-Front: Vue
-Back: JavaScript, Express, Node
-BD: SQL</t>
   </si>
   <si>
     <t>Creacion y configuracion cuenta Github tablero</t>
@@ -342,6 +321,20 @@
   </si>
   <si>
     <t>Asignar un veterinario a una mascota.</t>
+  </si>
+  <si>
+    <t>Front: html, css
+Back: C++
+BD: SQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración inicial </t>
+  </si>
+  <si>
+    <t>Construccion Inicial de MockUps</t>
+  </si>
+  <si>
+    <t>Construccion Historias de Usuario Sprint 1</t>
   </si>
 </sst>
 </file>
@@ -670,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -740,9 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -881,9 +871,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,21 +880,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -925,11 +897,26 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="107">
+  <dxfs count="77">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -952,526 +939,6 @@
           <fgColor rgb="FFCCFFCC"/>
           <bgColor rgb="FFCCFFCC"/>
         </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFCC"/>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF666699"/>
-      </font>
-      <fill>
-        <patternFill patternType="none"/>
       </fill>
     </dxf>
     <dxf>
@@ -1836,6 +1303,94 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2624,6 +2179,198 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666699"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2638,58 +2385,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F899EF04-071F-4438-9F03-C42B061D8F9E}" name="Tabla1" displayName="Tabla1" ref="A2:J10" totalsRowShown="0" headerRowDxfId="106" headerRowBorderDxfId="105" tableBorderDxfId="104" totalsRowBorderDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F899EF04-071F-4438-9F03-C42B061D8F9E}" name="Tabla1" displayName="Tabla1" ref="A2:J10" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50" totalsRowBorderDxfId="49">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{66CC9B29-972E-440A-912D-BD4A014746AB}" name="Incr." dataDxfId="102"/>
-    <tableColumn id="2" xr3:uid="{8DB82F78-68F3-42A2-850E-63D287D60F0F}" name="Start" dataDxfId="101"/>
-    <tableColumn id="3" xr3:uid="{F968D6EE-A810-4E1A-B390-2EB3FDF1FEBC}" name="Days" dataDxfId="100"/>
-    <tableColumn id="4" xr3:uid="{AAF044F0-1EF6-4F39-B0EC-7E4FF5284F1E}" name="End" dataDxfId="99"/>
-    <tableColumn id="5" xr3:uid="{43FD3FBC-D2AD-4693-A6D3-2D3C3CEA7764}" name="Estimated Size" dataDxfId="98"/>
-    <tableColumn id="6" xr3:uid="{845D7AAE-192D-4ACB-98F1-13E2AB396319}" name="Real Size" dataDxfId="97"/>
-    <tableColumn id="7" xr3:uid="{3A55337D-C59A-4152-AB89-7F958089BEB6}" name="Status" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{66CC9B29-972E-440A-912D-BD4A014746AB}" name="Incr." dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{8DB82F78-68F3-42A2-850E-63D287D60F0F}" name="Start" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{F968D6EE-A810-4E1A-B390-2EB3FDF1FEBC}" name="Days" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{AAF044F0-1EF6-4F39-B0EC-7E4FF5284F1E}" name="End" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{43FD3FBC-D2AD-4693-A6D3-2D3C3CEA7764}" name="Estimated Size" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{845D7AAE-192D-4ACB-98F1-13E2AB396319}" name="Real Size" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{3A55337D-C59A-4152-AB89-7F958089BEB6}" name="Status" dataDxfId="42"/>
     <tableColumn id="8" xr3:uid="{38918B64-CCE0-4636-A5E4-263FE5F24E44}" name="Release Date"/>
-    <tableColumn id="9" xr3:uid="{60143B17-7058-4AA2-BE5E-4B4A6B0F3F79}" name="Goal" dataDxfId="95"/>
-    <tableColumn id="10" xr3:uid="{08E89F60-45A7-4FE5-84CF-07185CF17579}" name="% Esfuerzo vs Estimación" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{60143B17-7058-4AA2-BE5E-4B4A6B0F3F79}" name="Goal" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{08E89F60-45A7-4FE5-84CF-07185CF17579}" name="% Esfuerzo vs Estimación" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6B9DA90-D87F-4F67-9EB9-B6BDCC070AB7}" name="Tabla2" displayName="Tabla2" ref="A13:K27" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6B9DA90-D87F-4F67-9EB9-B6BDCC070AB7}" name="Tabla2" displayName="Tabla2" ref="A13:K27" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3F7F6DD2-6EA2-4440-BD0B-88E2A12AF313}" name="Sprint" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{62768372-7E11-44D1-A207-F692349A3997}" name="Start" dataDxfId="89">
+    <tableColumn id="1" xr3:uid="{3F7F6DD2-6EA2-4440-BD0B-88E2A12AF313}" name="Sprint" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{62768372-7E11-44D1-A207-F692349A3997}" name="Start" dataDxfId="35">
       <calculatedColumnFormula>IF(AND(B13&lt;&gt;"",C13&lt;&gt;"",C14&lt;&gt;""),B13+C13,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F25C110E-5E39-4470-8BC8-391189A23F6A}" name="Days" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{B5697784-C933-4A45-8BA8-617CDCABE74D}" name="End" dataDxfId="87">
+    <tableColumn id="3" xr3:uid="{F25C110E-5E39-4470-8BC8-391189A23F6A}" name="Days" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{B5697784-C933-4A45-8BA8-617CDCABE74D}" name="End" dataDxfId="33">
       <calculatedColumnFormula>IF(AND(B14&lt;&gt;"",C14&lt;&gt;""),B14+C14-1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5518327B-86C2-485C-AF9A-553A341AB62F}" name="Estimated Size" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{8EE1AD7A-512C-42AD-9C83-F3DE570521F3}" name="Real Size" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{879F25EC-AE5A-403A-BB1E-715A98E973E5}" name="Status" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{35D9BAA4-D3E2-4602-BFEC-3D9FAF91D9FB}" name="Release Date" dataDxfId="83"/>
-    <tableColumn id="9" xr3:uid="{25759FDC-EAD4-41CE-B98D-B6CA5005C897}" name="Goal" dataDxfId="82"/>
-    <tableColumn id="10" xr3:uid="{767130C5-3778-4D2D-B165-AAC8557C9C26}" name="Increment" dataDxfId="81"/>
-    <tableColumn id="11" xr3:uid="{BB50C29E-17AE-4847-B617-C1464CB872F4}" name="% Error estimación" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{5518327B-86C2-485C-AF9A-553A341AB62F}" name="Estimated Size" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{8EE1AD7A-512C-42AD-9C83-F3DE570521F3}" name="Real Size" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{879F25EC-AE5A-403A-BB1E-715A98E973E5}" name="Status" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{35D9BAA4-D3E2-4602-BFEC-3D9FAF91D9FB}" name="Release Date" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{25759FDC-EAD4-41CE-B98D-B6CA5005C897}" name="Goal" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{767130C5-3778-4D2D-B165-AAC8557C9C26}" name="Increment" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{BB50C29E-17AE-4847-B617-C1464CB872F4}" name="% Error estimación" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55EDAA51-64A0-4C3C-BB05-C8B91F0B95A2}" name="Tabla3" displayName="Tabla3" ref="A2:I25" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{55EDAA51-64A0-4C3C-BB05-C8B91F0B95A2}" name="Tabla3" displayName="Tabla3" ref="A2:I25" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5C9319BF-6D02-43C9-BCA9-5EDBE9878A57}" name="Story ID" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{4C99E7E9-CEA2-43DA-87BD-F48F11ACCC65}" name="Story name" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{0A2A499E-9D5E-466D-A989-7A59E43BB357}" name="Status" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{5469DBC9-3DA2-4F4B-8710-F10B84BF1829}" name="Size" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{5305EA1B-B894-4B83-B24C-75E39016D04C}" name="Sprint" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{04E09A1B-DCFB-4289-8952-40AB55E5A7FA}" name="Priority" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{81D2D2DA-2F15-4682-AF3F-DDC36F5414A0}" name="Story Type" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{7448AE9C-D97B-4E61-83F8-FFB1973FA36F}" name="Comments" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{44E148DE-5F04-4CEE-9AAC-6230A237917E}" name="Additional Comments" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{5C9319BF-6D02-43C9-BCA9-5EDBE9878A57}" name="Story ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4C99E7E9-CEA2-43DA-87BD-F48F11ACCC65}" name="Story name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{0A2A499E-9D5E-466D-A989-7A59E43BB357}" name="Status" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{5469DBC9-3DA2-4F4B-8710-F10B84BF1829}" name="Size" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{5305EA1B-B894-4B83-B24C-75E39016D04C}" name="Sprint" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{04E09A1B-DCFB-4289-8952-40AB55E5A7FA}" name="Priority" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{81D2D2DA-2F15-4682-AF3F-DDC36F5414A0}" name="Story Type" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{7448AE9C-D97B-4E61-83F8-FFB1973FA36F}" name="Comments" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{44E148DE-5F04-4CEE-9AAC-6230A237917E}" name="Additional Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2896,7 +2643,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2916,90 +2663,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-    </row>
-    <row r="2" spans="1:26" s="72" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+    </row>
+    <row r="2" spans="1:26" s="71" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="69" t="s">
+      <c r="J2" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47">
+      <c r="A3" s="46">
         <v>1</v>
       </c>
       <c r="B3" s="4">
         <f>IF(OR(B14="",A3=""),"",B14)</f>
-        <v>44789</v>
+        <v>44799</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="45">
         <f>ROUND((SUMIF(A14:A21,A3,F14:F21)/8),0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D9" si="0">IF(OR(B3="",C3=""),"",B3+C3-1)</f>
-        <v>44793</v>
+        <v>44802</v>
       </c>
       <c r="E3" s="3">
         <f>IF(A3="","",SUMIF(J$14:J$29,'Release Plan'!A3,E$14:E$29))</f>
-        <v>36.300000000000004</v>
+        <v>44.300000000000004</v>
       </c>
       <c r="F3" s="3">
         <f>IF(A3="","",SUMIF(J$14:J$29,'Release Plan'!A3,F$14:F$29))</f>
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>38</v>
@@ -3010,13 +2757,13 @@
       <c r="I3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="49">
+      <c r="J3" s="48">
         <f>(F3/E3)</f>
-        <v>1.0743801652892562</v>
+        <v>1.1738148984198644</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="47"/>
+      <c r="A4" s="46"/>
       <c r="B4" s="4" t="str">
         <f t="shared" ref="B4:B8" si="1">IF(A4="","",B3+C3)</f>
         <v/>
@@ -3039,10 +2786,10 @@
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="49"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3065,10 +2812,10 @@
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="49"/>
+      <c r="J5" s="48"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3091,10 +2838,10 @@
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="49"/>
+      <c r="J6" s="48"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3117,10 +2864,10 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="49"/>
+      <c r="J7" s="48"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="48"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -3140,10 +2887,10 @@
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="49"/>
+      <c r="J8" s="48"/>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="48"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="str">
         <f>IF(A9="","",SUMIF(J$14:J$29,A9,C$14:C$29))</f>
@@ -3161,79 +2908,79 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="50"/>
+      <c r="J9" s="49"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="53"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="52"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:26" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
     </row>
     <row r="13" spans="1:26" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="68" t="s">
+      <c r="G13" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="67" t="s">
+      <c r="H13" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="69" t="s">
+      <c r="K13" s="68" t="s">
         <v>16</v>
       </c>
       <c r="L13" s="2"/>
@@ -3254,24 +3001,24 @@
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="12">
-        <v>44789</v>
+        <v>44799</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C14" s="44">
         <f>+F14*1/F$14</f>
         <v>1</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" ref="D14:D26" si="2">IF(AND(B14&lt;&gt;"",C14&lt;&gt;""),B14+C14-1,"")</f>
-        <v>44789</v>
+        <v>44799</v>
       </c>
       <c r="E14" s="5">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="F14" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>11</v>
@@ -3285,32 +3032,32 @@
       <c r="J14" s="3">
         <v>1</v>
       </c>
-      <c r="K14" s="49">
+      <c r="K14" s="48">
         <f>(F14/E14)-1</f>
-        <v>7.6923076923076872E-2</v>
+        <v>0.33333333333333326</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="4">
         <f>IF(AND(B14&lt;&gt;"",C14&lt;&gt;"",C15&lt;&gt;""),B14+C14,"")</f>
-        <v>44790</v>
+        <v>44800</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C15" s="44">
         <f t="shared" ref="C15:C21" si="3">+F15*1/F$14</f>
-        <v>0.2857142857142857</v>
+        <v>0.4</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="2"/>
-        <v>44789.285714285717</v>
+        <v>44799.4</v>
       </c>
       <c r="E15" s="3">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="F15" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>11</v>
@@ -3324,32 +3071,32 @@
       <c r="J15" s="3">
         <v>1</v>
       </c>
-      <c r="K15" s="49">
+      <c r="K15" s="48">
         <f t="shared" ref="K15:K21" si="4">(F15/E15)-1</f>
-        <v>0.11111111111111116</v>
+        <v>0.4285714285714286</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" ref="B15:B26" si="5">IF(AND(B15&lt;&gt;"",C15&lt;&gt;"",C16&lt;&gt;""),B15+C15,"")</f>
-        <v>44790.285714285717</v>
+        <f t="shared" ref="B16:B26" si="5">IF(AND(B15&lt;&gt;"",C15&lt;&gt;"",C16&lt;&gt;""),B15+C15,"")</f>
+        <v>44800.4</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C16" s="44">
         <f t="shared" si="3"/>
-        <v>0.42857142857142855</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="2"/>
-        <v>44789.71428571429</v>
+        <v>44799.9</v>
       </c>
       <c r="E16" s="3">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
       <c r="F16" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>11</v>
@@ -3363,9 +3110,9 @@
       <c r="J16" s="3">
         <v>1</v>
       </c>
-      <c r="K16" s="49">
+      <c r="K16" s="48">
         <f t="shared" si="4"/>
-        <v>7.1428571428571397E-2</v>
+        <v>0.31578947368421062</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3373,22 +3120,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" si="5"/>
-        <v>44790.71428571429</v>
+        <f>IF(AND(B16&lt;&gt;"",C16&lt;&gt;"",C17&lt;&gt;""),B16+C16,"")</f>
+        <v>44800.9</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="44">
         <f t="shared" si="3"/>
-        <v>0.42857142857142855</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="2"/>
-        <v>44790.142857142862</v>
+        <v>44800.4</v>
       </c>
       <c r="E17" s="3">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>38</v>
@@ -3402,9 +3149,9 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="K17" s="49">
+      <c r="K17" s="48">
         <f t="shared" si="4"/>
-        <v>0.11111111111111094</v>
+        <v>0.35135135135135132</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3413,21 +3160,21 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" si="5"/>
-        <v>44791.142857142862</v>
+        <v>44801.4</v>
       </c>
-      <c r="C18" s="45">
+      <c r="C18" s="44">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="2"/>
-        <v>44791.142857142862</v>
+        <v>44801.200000000004</v>
       </c>
       <c r="E18" s="5">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
       <c r="F18" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>38</v>
@@ -3441,9 +3188,9 @@
       <c r="J18" s="3">
         <v>1</v>
       </c>
-      <c r="K18" s="49">
+      <c r="K18" s="48">
         <f t="shared" si="4"/>
-        <v>2.941176470588247E-2</v>
+        <v>2.5641025641025772E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3452,21 +3199,21 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" si="5"/>
-        <v>44792.142857142862</v>
+        <v>44802.200000000004</v>
       </c>
-      <c r="C19" s="45">
+      <c r="C19" s="44">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="2"/>
-        <v>44792.142857142862</v>
+        <v>44802.000000000007</v>
       </c>
       <c r="E19" s="5">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
       <c r="F19" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>36</v>
@@ -3480,9 +3227,9 @@
       <c r="J19" s="3">
         <v>1</v>
       </c>
-      <c r="K19" s="49">
+      <c r="K19" s="48">
         <f t="shared" si="4"/>
-        <v>6.0606060606060552E-2</v>
+        <v>5.2631578947368363E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3491,21 +3238,21 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" si="5"/>
-        <v>44793.142857142862</v>
+        <v>44803.000000000007</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="44">
         <f t="shared" si="3"/>
-        <v>0.7142857142857143</v>
+        <v>0.6</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>44792.857142857145</v>
+        <v>44802.600000000006</v>
       </c>
       <c r="E20" s="5">
-        <v>4.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="F20" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>36</v>
@@ -3519,9 +3266,9 @@
       <c r="J20" s="5">
         <v>1</v>
       </c>
-      <c r="K20" s="49">
+      <c r="K20" s="48">
         <f t="shared" si="4"/>
-        <v>8.6956521739130599E-2</v>
+        <v>7.1428571428571397E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3530,21 +3277,21 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" si="5"/>
-        <v>44793.857142857145</v>
+        <v>44803.600000000006</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="44">
         <f t="shared" si="3"/>
-        <v>0.7142857142857143</v>
+        <v>0.6</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>44793.571428571428</v>
+        <v>44803.200000000004</v>
       </c>
       <c r="E21" s="5">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F21" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>36</v>
@@ -3552,15 +3299,13 @@
       <c r="H21" s="7">
         <v>44449</v>
       </c>
-      <c r="I21" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="I21" s="15"/>
       <c r="J21" s="5">
         <v>1</v>
       </c>
-      <c r="K21" s="49">
+      <c r="K21" s="48">
         <f t="shared" si="4"/>
-        <v>0.11111111111111116</v>
+        <v>9.0909090909090828E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3581,7 +3326,7 @@
       </c>
       <c r="H22" s="7"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="55"/>
+      <c r="K22" s="54"/>
     </row>
     <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
@@ -3602,7 +3347,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="16"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="55"/>
+      <c r="K23" s="54"/>
     </row>
     <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
@@ -3682,66 +3427,66 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="56"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="66"/>
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="65"/>
     </row>
     <row r="30" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="89" t="s">
-        <v>46</v>
+      <c r="A30" s="92" t="s">
+        <v>43</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="89"/>
-      <c r="D30" s="89"/>
-      <c r="E30" s="75">
+      <c r="B30" s="92"/>
+      <c r="C30" s="92"/>
+      <c r="D30" s="92"/>
+      <c r="E30" s="74">
         <f>SUMIF('Product Backlog'!E$3:E$74,"",'Product Backlog'!D$3:D$74)-SUMIF('Product Backlog'!C$3:C$74,"Removed",'Product Backlog'!D$3:D$74)</f>
         <v>0</v>
       </c>
-      <c r="F30" s="75"/>
+      <c r="F30" s="74"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="62"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="61"/>
     </row>
     <row r="31" spans="1:12" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="88" t="s">
+      <c r="A31" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="88"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="75">
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="74">
         <f>SUM(E14:E29)</f>
-        <v>36.300000000000004</v>
+        <v>44.300000000000004</v>
       </c>
-      <c r="F31" s="75">
+      <c r="F31" s="74">
         <f>SUM(F14:F29)</f>
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:12" s="73" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E32" s="76" t="s">
-        <v>47</v>
+    <row r="32" spans="1:12" s="72" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E32" s="75" t="s">
+        <v>44</v>
       </c>
-      <c r="F32" s="76" t="s">
-        <v>48</v>
+      <c r="F32" s="75" t="s">
+        <v>45</v>
       </c>
-      <c r="H32" s="74"/>
+      <c r="H32" s="73"/>
     </row>
     <row r="33" spans="4:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D33" s="18"/>
@@ -6655,122 +6400,122 @@
     <mergeCell ref="A30:D30"/>
   </mergeCells>
   <conditionalFormatting sqref="H3:I8 E4:F8 E30:F31 A3:D8 F5:I5">
-    <cfRule type="expression" dxfId="67" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="13" stopIfTrue="1">
       <formula>$G2="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I8 E4:F8 E30:F31 A3:D8 F5:I5">
-    <cfRule type="expression" dxfId="66" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="14" stopIfTrue="1">
       <formula>$G2="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 G14:G23 G29">
-    <cfRule type="expression" dxfId="65" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="15" stopIfTrue="1">
       <formula>$G3="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 H14:I16 H23:I23 I17:I21 G14:G23 H15:H22 G29:I29">
-    <cfRule type="expression" dxfId="64" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="16" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G8 G14:G23 G29">
-    <cfRule type="cellIs" dxfId="63" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="17" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4 F3:F7 H3:H7 H14:I16 H23:I23 H15:H22 B14:F23 H29:I29 A29:F29">
-    <cfRule type="expression" dxfId="62" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="18" stopIfTrue="1">
       <formula>OR($G3="Planned",$G3="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E4 F3:F7 H3:H7 B14:F23 A29:F29">
-    <cfRule type="expression" dxfId="61" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="60" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="20" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="59" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="58" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B23">
-    <cfRule type="expression" dxfId="57" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D23">
-    <cfRule type="expression" dxfId="56" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
       <formula>$G14="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:D23">
-    <cfRule type="expression" dxfId="55" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="25" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:I21">
-    <cfRule type="expression" dxfId="54" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="34" stopIfTrue="1">
       <formula>OR($G17="Planned",$G17="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:J10">
-    <cfRule type="expression" dxfId="53" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="11" stopIfTrue="1">
       <formula>$G9="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:J10">
-    <cfRule type="expression" dxfId="52" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="12" stopIfTrue="1">
       <formula>$G9="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:J9">
-    <cfRule type="expression" dxfId="51" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="9" stopIfTrue="1">
       <formula>$G8="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:J9">
-    <cfRule type="expression" dxfId="50" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="10" stopIfTrue="1">
       <formula>$G8="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:J11">
-    <cfRule type="expression" dxfId="49" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="7" stopIfTrue="1">
       <formula>$G10="Planned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:J11">
-    <cfRule type="expression" dxfId="48" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="8" stopIfTrue="1">
       <formula>$G10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A23">
-    <cfRule type="expression" dxfId="47" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="5" stopIfTrue="1">
       <formula>OR($G14="Planned",$G14="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:K28">
-    <cfRule type="expression" dxfId="46" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="1" stopIfTrue="1">
       <formula>OR($G24="Planned",$G24="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A23">
-    <cfRule type="expression" dxfId="45" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="6" stopIfTrue="1">
       <formula>$G14="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:K28">
-    <cfRule type="expression" dxfId="44" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="2" stopIfTrue="1">
       <formula>$G24="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6796,34 +6541,34 @@
   <dimension ref="A1:Z981"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="A10:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="2" max="2" width="111" customWidth="1"/>
+    <col min="2" max="2" width="105.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="47" customWidth="1"/>
     <col min="9" max="9" width="46.140625" customWidth="1"/>
     <col min="10" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
       <c r="L1" s="24"/>
@@ -6843,31 +6588,31 @@
       <c r="Z1" s="24"/>
     </row>
     <row r="2" spans="1:26" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="D2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="82" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="24"/>
@@ -6899,7 +6644,7 @@
         <v>33</v>
       </c>
       <c r="D3" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" s="25">
         <v>0</v>
@@ -6911,9 +6656,9 @@
         <v>34</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
-      <c r="I3" s="32"/>
+      <c r="I3" s="31"/>
       <c r="J3" s="24"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
@@ -6936,14 +6681,14 @@
       <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="87" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="28">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="25">
         <v>0</v>
@@ -6957,7 +6702,7 @@
       <c r="H4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="32"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="24"/>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
@@ -6976,11 +6721,11 @@
       <c r="Y4" s="24"/>
       <c r="Z4" s="24"/>
     </row>
-    <row r="5" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="87" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="27" t="s">
@@ -6999,9 +6744,9 @@
         <v>34</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
-      <c r="I5" s="32"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="24"/>
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
@@ -7024,7 +6769,7 @@
       <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="87" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -7043,9 +6788,9 @@
         <v>34</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
@@ -7068,8 +6813,8 @@
       <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="94" t="s">
-        <v>57</v>
+      <c r="B7" s="87" t="s">
+        <v>51</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>33</v>
@@ -7087,9 +6832,9 @@
         <v>34</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
@@ -7112,8 +6857,8 @@
       <c r="A8" s="25">
         <v>6</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>22</v>
+      <c r="B8" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>33</v>
@@ -7131,9 +6876,9 @@
         <v>34</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
@@ -7156,8 +6901,8 @@
       <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>44</v>
+      <c r="B9" s="30" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>33</v>
@@ -7175,11 +6920,11 @@
         <v>34</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
-      <c r="I9" s="32"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="24"/>
-      <c r="K9" s="33"/>
+      <c r="K9" s="32"/>
       <c r="L9" s="24"/>
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
@@ -7197,703 +6942,771 @@
       <c r="Z9" s="24"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34">
+      <c r="A10" s="33">
         <v>9</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>54</v>
+      <c r="B10" s="30" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="28">
         <v>3</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="33">
         <v>2</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="33">
         <v>2</v>
       </c>
-      <c r="G10" s="78" t="s">
-        <v>49</v>
+      <c r="G10" s="77" t="s">
+        <v>46</v>
       </c>
-      <c r="H10" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="80"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="36"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="36"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="36"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="35"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="34">
+      <c r="A11" s="33">
         <v>10</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>68</v>
+      <c r="B11" s="30" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="28">
         <v>6</v>
       </c>
-      <c r="E11" s="34">
+      <c r="E11" s="33">
         <v>2</v>
       </c>
-      <c r="F11" s="77"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="82" t="s">
-        <v>51</v>
+      <c r="F11" s="33">
+        <v>2</v>
       </c>
-      <c r="I11" s="82"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="36"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="36"/>
-      <c r="Z11" s="36"/>
+      <c r="G11" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="35"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="33">
         <v>11</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>52</v>
+      <c r="B12" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="28">
         <v>5</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <v>2</v>
       </c>
-      <c r="F12" s="77"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="82" t="s">
-        <v>51</v>
+      <c r="F12" s="33">
+        <v>2</v>
       </c>
-      <c r="I12" s="82"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
+      <c r="G12" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="35"/>
     </row>
     <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="34">
+      <c r="A13" s="33">
         <v>12</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>53</v>
+      <c r="B13" s="30" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D13" s="28">
         <v>3</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <v>2</v>
       </c>
-      <c r="F13" s="77"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82" t="s">
-        <v>51</v>
+      <c r="F13" s="33">
+        <v>2</v>
       </c>
-      <c r="I13" s="82"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="36"/>
+      <c r="G13" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="80"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
+      <c r="X13" s="35"/>
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="35"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="34">
+      <c r="A14" s="33">
         <v>13</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>55</v>
+      <c r="B14" s="30" t="s">
+        <v>50</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" s="28">
         <v>3</v>
       </c>
-      <c r="E14" s="34">
+      <c r="E14" s="33">
         <v>2</v>
       </c>
-      <c r="F14" s="77"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="82" t="s">
-        <v>51</v>
+      <c r="F14" s="33">
+        <v>2</v>
       </c>
-      <c r="I14" s="82"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
+      <c r="G14" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="34">
+      <c r="A15" s="33">
         <v>14</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>58</v>
+      <c r="B15" s="30" t="s">
+        <v>52</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D15" s="28">
         <v>5</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="33">
         <v>3</v>
       </c>
-      <c r="F15" s="77"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="82" t="s">
-        <v>51</v>
+      <c r="F15" s="76">
+        <v>1</v>
       </c>
-      <c r="I15" s="82"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="36"/>
+      <c r="G15" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="35"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="34">
+      <c r="A16" s="33">
         <v>15</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>59</v>
+      <c r="B16" s="30" t="s">
+        <v>53</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D16" s="28">
         <v>8</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="33">
         <v>3</v>
       </c>
-      <c r="F16" s="77"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="82" t="s">
-        <v>51</v>
+      <c r="F16" s="76">
+        <v>1</v>
       </c>
-      <c r="I16" s="82"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
-      <c r="S16" s="36"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="36"/>
-      <c r="W16" s="36"/>
-      <c r="X16" s="36"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
+      <c r="G16" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="35"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
+      <c r="A17" s="33">
         <v>16</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>60</v>
+      <c r="B17" s="30" t="s">
+        <v>54</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D17" s="28">
         <v>8</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="33">
         <v>3</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
+      <c r="F17" s="76">
+        <v>1</v>
+      </c>
+      <c r="G17" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="84"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34">
+      <c r="A18" s="33">
         <v>17</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>61</v>
+      <c r="B18" s="30" t="s">
+        <v>55</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D18" s="28">
         <v>8</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="33">
         <v>3</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
+      <c r="F18" s="76">
+        <v>1</v>
+      </c>
+      <c r="G18" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="84"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="35"/>
+      <c r="U18" s="35"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="35"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34">
+      <c r="A19" s="33">
         <v>18</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>62</v>
+      <c r="B19" s="30" t="s">
+        <v>56</v>
       </c>
-      <c r="C19" s="35"/>
+      <c r="C19" s="34" t="s">
+        <v>38</v>
+      </c>
       <c r="D19" s="28">
         <v>5</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="33">
         <v>3</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="36"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="36"/>
-      <c r="W19" s="36"/>
-      <c r="X19" s="36"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
+      <c r="F19" s="76">
+        <v>1</v>
+      </c>
+      <c r="G19" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="84"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="35"/>
+      <c r="Q19" s="35"/>
+      <c r="R19" s="35"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="35"/>
+      <c r="U19" s="35"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
+      <c r="X19" s="35"/>
+      <c r="Y19" s="35"/>
+      <c r="Z19" s="35"/>
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="78">
+      <c r="A20" s="77">
         <v>19</v>
       </c>
-      <c r="B20" s="92" t="s">
-        <v>69</v>
+      <c r="B20" s="85" t="s">
+        <v>63</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D20" s="28">
         <v>8</v>
       </c>
-      <c r="E20" s="78">
+      <c r="E20" s="77">
         <v>4</v>
       </c>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="36"/>
+      <c r="F20" s="77">
+        <v>2</v>
+      </c>
+      <c r="G20" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="84"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="35"/>
+      <c r="Z20" s="35"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="78">
+      <c r="A21" s="77">
         <v>20</v>
       </c>
-      <c r="B21" s="92" t="s">
-        <v>63</v>
+      <c r="B21" s="85" t="s">
+        <v>57</v>
       </c>
-      <c r="C21" s="93"/>
+      <c r="C21" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D21" s="28">
         <v>8</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="77">
         <v>4</v>
       </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="36"/>
+      <c r="F21" s="77">
+        <v>2</v>
+      </c>
+      <c r="G21" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="84"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="35"/>
+      <c r="Z21" s="35"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="78">
+      <c r="A22" s="77">
         <v>21</v>
       </c>
-      <c r="B22" s="92" t="s">
-        <v>64</v>
+      <c r="B22" s="85" t="s">
+        <v>58</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D22" s="28">
         <v>8</v>
       </c>
-      <c r="E22" s="78">
+      <c r="E22" s="77">
         <v>4</v>
       </c>
-      <c r="F22" s="78"/>
-      <c r="G22" s="78"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
+      <c r="F22" s="77">
+        <v>2</v>
+      </c>
+      <c r="G22" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="84"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="78">
+      <c r="A23" s="77">
         <v>22</v>
       </c>
-      <c r="B23" s="95" t="s">
-        <v>65</v>
+      <c r="B23" s="88" t="s">
+        <v>59</v>
       </c>
-      <c r="C23" s="93"/>
+      <c r="C23" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D23" s="28">
         <v>8</v>
       </c>
-      <c r="E23" s="78">
+      <c r="E23" s="77">
         <v>4</v>
       </c>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
+      <c r="F23" s="77">
+        <v>2</v>
+      </c>
+      <c r="G23" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="84"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35"/>
+      <c r="Y23" s="35"/>
+      <c r="Z23" s="35"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="78">
+      <c r="A24" s="77">
         <v>23</v>
       </c>
-      <c r="B24" s="92" t="s">
-        <v>66</v>
+      <c r="B24" s="85" t="s">
+        <v>60</v>
       </c>
-      <c r="C24" s="93"/>
+      <c r="C24" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D24" s="28">
         <v>8</v>
       </c>
-      <c r="E24" s="78">
+      <c r="E24" s="77">
         <v>4</v>
       </c>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
+      <c r="F24" s="77">
+        <v>2</v>
+      </c>
+      <c r="G24" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="84"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="78">
+      <c r="A25" s="77">
         <v>24</v>
       </c>
-      <c r="B25" s="92" t="s">
-        <v>67</v>
+      <c r="B25" s="85" t="s">
+        <v>61</v>
       </c>
-      <c r="C25" s="93"/>
+      <c r="C25" s="86" t="s">
+        <v>36</v>
+      </c>
       <c r="D25" s="28">
         <v>8</v>
       </c>
-      <c r="E25" s="78">
+      <c r="E25" s="77">
         <v>4</v>
       </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
-      <c r="P25" s="36"/>
-      <c r="Q25" s="36"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="36"/>
-      <c r="U25" s="36"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="36"/>
-      <c r="X25" s="36"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="36"/>
+      <c r="F25" s="77">
+        <v>2</v>
+      </c>
+      <c r="G25" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="84"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
+      <c r="X25" s="35"/>
+      <c r="Y25" s="35"/>
+      <c r="Z25" s="35"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="36"/>
-      <c r="U26" s="36"/>
-      <c r="V26" s="36"/>
-      <c r="W26" s="36"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="36"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="35"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="36"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="36"/>
-      <c r="W27" s="36"/>
-      <c r="X27" s="36"/>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="36"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="35"/>
+      <c r="Y27" s="35"/>
+      <c r="Z27" s="35"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="36"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="36"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="35"/>
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
@@ -7913,15 +7726,15 @@
       <c r="Z29" s="24"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="40"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="36"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="35"/>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
@@ -7941,15 +7754,15 @@
       <c r="Z30" s="24"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="36"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="35"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
@@ -7969,15 +7782,15 @@
       <c r="Z31" s="24"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="36"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="35"/>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
@@ -7997,15 +7810,15 @@
       <c r="Z32" s="24"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="36"/>
+      <c r="A33" s="38"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="41"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="35"/>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
@@ -8025,15 +7838,15 @@
       <c r="Z33" s="24"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="36"/>
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="35"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
@@ -8053,15 +7866,15 @@
       <c r="Z34" s="24"/>
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="36"/>
+      <c r="A35" s="38"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="35"/>
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
@@ -8081,14 +7894,14 @@
       <c r="Z35" s="24"/>
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
       <c r="G36" s="23"/>
-      <c r="H36" s="44"/>
+      <c r="H36" s="43"/>
       <c r="I36" s="24"/>
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
@@ -8137,14 +7950,14 @@
       <c r="Z37" s="24"/>
     </row>
     <row r="38" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="43"/>
-      <c r="B38" s="44"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="22"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="23"/>
-      <c r="H38" s="44"/>
+      <c r="H38" s="43"/>
       <c r="I38" s="24"/>
       <c r="J38" s="24"/>
       <c r="K38" s="24"/>
@@ -34454,72 +34267,72 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B25">
-    <cfRule type="expression" dxfId="43" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
       <formula>OR($G3="Planned",$G3="Unplanned")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B25">
-    <cfRule type="expression" dxfId="42" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
       <formula>$G3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9 A27:H981 H10:I10 I2:I10 A2:G25">
-    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9 A27:H981 H10:I10 I2:I10 A2:G25">
-    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9 A27:H981 H10:I10 I2:I10 A2:G25">
-    <cfRule type="expression" dxfId="39" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="expression" dxfId="38" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="6" stopIfTrue="1">
       <formula>$C3="Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="expression" dxfId="37" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
       <formula>$C3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I10">
-    <cfRule type="expression" dxfId="36" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="8" stopIfTrue="1">
       <formula>$C3="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="35" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="9" stopIfTrue="1">
       <formula>$C3="Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="34" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
       <formula>$C3="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="expression" dxfId="33" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="11" stopIfTrue="1">
       <formula>$C3="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="32" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="12" stopIfTrue="1">
       <formula>$C5="Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="13" stopIfTrue="1">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="30" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="14" stopIfTrue="1">
       <formula>$C5="Removed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>